<commit_message>
fixed reset line, added current-limiting resistor and bypass cap
</commit_message>
<xml_diff>
--- a/Sprite_BOM.xlsx
+++ b/Sprite_BOM.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-20" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="sprite" localSheetId="0">Sheet1!$A$6:$G$27</definedName>
+    <definedName name="sprite" localSheetId="0">Sheet1!$A$6:$G$26</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="131">
   <si>
     <t>Qty</t>
   </si>
@@ -146,12 +146,6 @@
     <t>Inductors</t>
   </si>
   <si>
-    <t>2.2nF</t>
-  </si>
-  <si>
-    <t>C13</t>
-  </si>
-  <si>
     <t>2.7V</t>
   </si>
   <si>
@@ -326,9 +320,6 @@
     <t>478-5167-2-ND</t>
   </si>
   <si>
-    <t>478-3615-2-ND</t>
-  </si>
-  <si>
     <t>478-1403-2-ND</t>
   </si>
   <si>
@@ -393,9 +384,6 @@
   </si>
   <si>
     <t>Pulse Electronics Corp.</t>
-  </si>
-  <si>
-    <t>08055F222K4T2A</t>
   </si>
   <si>
     <t>PDZ2.7B,115</t>
@@ -531,7 +519,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -557,6 +545,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -603,7 +592,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="24"/>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="49">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -639,6 +628,7 @@
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -984,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1004,17 +994,17 @@
   <sheetData>
     <row r="1" spans="1:9" s="8" customFormat="1">
       <c r="B1" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="B2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="B3" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1037,13 +1027,13 @@
         <v>5</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1051,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
@@ -1066,13 +1056,13 @@
         <v>9</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="13" t="s">
         <v>105</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1080,7 +1070,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
@@ -1095,13 +1085,13 @@
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1109,7 +1099,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -1121,16 +1111,16 @@
         <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1153,13 +1143,13 @@
         <v>20</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1170,7 +1160,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D11" s="11">
         <v>805</v>
@@ -1182,13 +1172,13 @@
         <v>24</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1211,13 +1201,13 @@
         <v>20</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1240,13 +1230,13 @@
         <v>20</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1269,13 +1259,13 @@
         <v>33</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1286,54 +1276,54 @@
         <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="11">
-        <v>805</v>
+        <v>98</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I15" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="D16" s="11">
+        <v>805</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I16" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1344,7 +1334,7 @@
         <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D17" s="11">
         <v>805</v>
@@ -1353,132 +1343,132 @@
         <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>95</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>2</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="11">
-        <v>805</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="I18" t="s">
-        <v>112</v>
+      <c r="F18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="2">
-        <v>2</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="D19" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>79</v>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I19" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>88</v>
+        <v>51</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>88</v>
+        <v>119</v>
       </c>
       <c r="I20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
         <v>52</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1486,100 +1476,100 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>55</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23">
         <v>1</v>
       </c>
-      <c r="B23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F23" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I23" t="s">
-        <v>128</v>
+      <c r="F23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24">
         <v>1</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="2" t="s">
+      <c r="D24" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="J24" s="2" t="s">
+      <c r="E24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>79</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="I24" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>62</v>
@@ -1588,74 +1578,45 @@
         <v>63</v>
       </c>
       <c r="F25" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="2">
+        <v>4</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G25" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="I25" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="B26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" t="s">
-        <v>73</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I26" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="2">
-        <v>4</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>79</v>
+      <c r="G26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>